<commit_message>
feat: Update RunPayrollDialog to use new API endpoint and improve form handling
- Refactored RunPayrollDialog component to remove unused form state and error handling.
- Changed API endpoint from /payroll/initiate-run to /payroll/calculate-run.
- Simplified form submission logic and removed redundant error messages.
- Updated PayrollPage to manage progress dialog state and handle rerun initiation.
- Added Accordion component for better UI organization.
- Updated API_BASE_URL to point to production server.
</commit_message>
<xml_diff>
--- a/public/assets/employee_import_template.xlsx
+++ b/public/assets/employee_import_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Documents\Clients\wagewise\wagewise-app\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3B3A9D-8C19-4DC4-BB65-EAFB59DD5FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB254A1D-3608-455B-BD0D-02856DFCE889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t>employee_number</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>punkzebra777@gmail.com</t>
+  </si>
+  <si>
+    <t>[{"type": "Housing ", "value": 15, "calculation_type": "Percentage"}]</t>
   </si>
 </sst>
 </file>
@@ -716,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="BE9" sqref="BE9"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +728,7 @@
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" customWidth="1"/>
     <col min="30" max="30" width="24.85546875" customWidth="1"/>
+    <col min="37" max="37" width="50.28515625" customWidth="1"/>
     <col min="47" max="47" width="15.5703125" customWidth="1"/>
     <col min="48" max="48" width="35.5703125" customWidth="1"/>
   </cols>
@@ -1011,8 +1015,8 @@
       <c r="AJ2" t="b">
         <v>1</v>
       </c>
-      <c r="AK2" t="b">
-        <v>1</v>
+      <c r="AK2" t="s">
+        <v>109</v>
       </c>
       <c r="AL2" t="b">
         <v>0</v>
@@ -1184,8 +1188,8 @@
       <c r="AJ3" t="b">
         <v>0</v>
       </c>
-      <c r="AK3" t="b">
-        <v>0</v>
+      <c r="AK3" t="s">
+        <v>109</v>
       </c>
       <c r="AL3" t="b">
         <v>0</v>

</xml_diff>